<commit_message>
Data That Needs To Be Uploaded Initially
</commit_message>
<xml_diff>
--- a/timeTabular-structure.xlsx
+++ b/timeTabular-structure.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\OneDrive\Desktop\TimeTabular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A05F68-058C-48EE-9943-0E79EBB6FD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B2F660-B662-4938-832C-1881F4EF8399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7237B49F-F46B-456A-897D-88F29124384A}"/>
   </bookViews>
@@ -534,28 +534,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC8B9EF-0AD2-4E19-A2AB-A8D1B65202A4}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
     <col min="10" max="10" width="8.33203125" customWidth="1"/>
     <col min="11" max="11" width="7.6640625" customWidth="1"/>
     <col min="12" max="12" width="9.44140625" customWidth="1"/>
     <col min="13" max="13" width="8.109375" customWidth="1"/>
     <col min="14" max="14" width="12.109375" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" customWidth="1"/>
-    <col min="16" max="16" width="14.109375" customWidth="1"/>
-    <col min="17" max="17" width="12.77734375" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" customWidth="1"/>
+    <col min="16" max="16" width="13.44140625" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>